<commit_message>
TestVer1.3 - enable multi ecid rows
</commit_message>
<xml_diff>
--- a/ECID report sample and Prouduct table template.xlsx
+++ b/ECID report sample and Prouduct table template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewECIDcheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267745CF-EAD0-4127-AFAB-6F3F5EFA556A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D00B2-C686-4FAD-929A-25D6EF9BBA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{5F970826-4D46-48D7-84A9-B3F6AF44BCAC}"/>
   </bookViews>
@@ -3251,12 +3251,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3266,17 +3260,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3844,7 +3844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD94CA40-2606-47F9-B3B0-DD79C54D4001}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -11073,37 +11073,37 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>273</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>866</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="37" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="40"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A5" s="41"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>67</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -11117,7 +11117,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="40"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="10" t="s">
         <v>224</v>
       </c>
@@ -11129,7 +11129,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A8" s="41"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="11" t="s">
         <v>225</v>
       </c>
@@ -11137,80 +11137,80 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>229</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="40" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="40"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="40"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A12" s="41"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="43" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="40"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="40"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
     </row>
     <row r="16" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A16" s="41"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:4" ht="14.5" thickBot="1">
       <c r="A17" s="15" t="s">
@@ -11269,51 +11269,51 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="43" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A22" s="41"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="43" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A24" s="41"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="38"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="44"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -11327,7 +11327,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A26" s="41"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="14" t="s">
         <v>225</v>
       </c>
@@ -11339,7 +11339,7 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="37" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -11353,7 +11353,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A28" s="41"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="14" t="s">
         <v>225</v>
       </c>
@@ -11365,83 +11365,82 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>244</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="43" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A30" s="38"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="43" t="s">
         <v>245</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="43" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A32" s="38"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="43" t="s">
         <v>246</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="43" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.5" thickBot="1">
-      <c r="A34" s="38"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
@@ -11456,12 +11455,13 @@
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>